<commit_message>
SMOTE update -> SMOTE + Threshold finalized.
</commit_message>
<xml_diff>
--- a/FinalResult.xlsx
+++ b/FinalResult.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haha9\Documents\GitHub\quantum-flakiness-ml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C709BEF4-952B-48E9-BE01-51F9BDA8978E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB623DE-E2AB-4D41-BDC5-5BADBB29CE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7590" yWindow="1920" windowWidth="13890" windowHeight="12780" xr2:uid="{0E69FEF2-CCF4-4F55-9C28-0EACB98F1DEB}"/>
+    <workbookView xWindow="8385" yWindow="1920" windowWidth="17805" windowHeight="12780" xr2:uid="{0E69FEF2-CCF4-4F55-9C28-0EACB98F1DEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="19">
   <si>
     <t>Model</t>
   </si>
@@ -77,21 +77,6 @@
     <t>MCC</t>
   </si>
   <si>
-    <t>equal Decision Tree</t>
-  </si>
-  <si>
-    <t>equal KNN</t>
-  </si>
-  <si>
-    <t>equal Random Forest</t>
-  </si>
-  <si>
-    <t>equal SVM</t>
-  </si>
-  <si>
-    <t>equal XGBoost</t>
-  </si>
-  <si>
     <t>Threshold only</t>
   </si>
   <si>
@@ -108,6 +93,9 @@
   </si>
   <si>
     <t>Regular model -Imbalance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XGBoost</t>
   </si>
 </sst>
 </file>
@@ -565,7 +553,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,59 +591,59 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.90300000000000002</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="C3">
-        <v>0.66500000000000004</v>
+        <v>0.89800000000000002</v>
       </c>
       <c r="D3">
-        <v>0.75600000000000001</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="E3" s="1">
-        <v>0.70499999999999996</v>
+        <v>0.876</v>
       </c>
       <c r="F3">
-        <v>0.65100000000000002</v>
+        <v>0.86299999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>0.91300000000000003</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="C4">
-        <v>0.81299999999999994</v>
+        <v>0.89400000000000002</v>
       </c>
       <c r="D4">
-        <v>0.57799999999999996</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="E4" s="2">
-        <v>0.66300000000000003</v>
+        <v>0.84199999999999997</v>
       </c>
       <c r="F4">
-        <v>0.63500000000000001</v>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>0.94799999999999995</v>
+        <v>0.89900000000000002</v>
       </c>
       <c r="C5">
-        <v>0.86399999999999999</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="D5">
-        <v>0.8</v>
+        <v>0.55600000000000005</v>
       </c>
       <c r="E5" s="3">
-        <v>0.82199999999999995</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="F5">
-        <v>0.79800000000000004</v>
+        <v>0.58599999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -663,19 +651,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="7">
-        <v>0.92700000000000005</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="C6" s="7">
-        <v>0.78200000000000003</v>
+        <v>0.82</v>
       </c>
       <c r="D6" s="7">
-        <v>0.75600000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="E6" s="8">
-        <v>0.76</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="F6" s="7">
-        <v>0.72299999999999998</v>
+        <v>0.76800000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -683,24 +671,24 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="C7">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="D7">
         <v>0.73299999999999998</v>
       </c>
-      <c r="D7">
-        <v>0.77300000000000002</v>
-      </c>
       <c r="E7" s="5">
-        <v>0.74199999999999999</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="F7">
-        <v>0.70299999999999996</v>
+        <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -728,59 +716,59 @@
         <v>4</v>
       </c>
       <c r="B12" s="7">
-        <v>0.78900000000000003</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="C12" s="7">
-        <v>0.77100000000000002</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="D12" s="7">
-        <v>0.84399999999999997</v>
+        <v>0.86699999999999999</v>
       </c>
       <c r="E12" s="9">
-        <v>0.79800000000000004</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="F12" s="7">
-        <v>0.59699999999999998</v>
+        <v>0.80500000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B13" s="7">
-        <v>0.74399999999999999</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="C13" s="7">
-        <v>0.872</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="D13" s="7">
-        <v>0.6</v>
+        <v>0.91100000000000003</v>
       </c>
       <c r="E13" s="10">
-        <v>0.69</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="F13" s="7">
-        <v>0.52600000000000002</v>
+        <v>0.78800000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B14" s="7">
-        <v>0.86699999999999999</v>
+        <v>0.74399999999999999</v>
       </c>
       <c r="C14" s="7">
-        <v>0.93100000000000005</v>
+        <v>0.872</v>
       </c>
       <c r="D14" s="7">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="E14" s="11">
-        <v>0.85</v>
+        <v>0.69</v>
       </c>
       <c r="F14" s="7">
-        <v>0.751</v>
+        <v>0.52500000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -805,27 +793,27 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B16" s="7">
-        <v>0.73599999999999999</v>
+        <v>0.755</v>
       </c>
       <c r="C16" s="7">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="D16" s="7">
         <v>0.82199999999999995</v>
       </c>
-      <c r="D16" s="7">
-        <v>0.76700000000000002</v>
-      </c>
       <c r="E16" s="12">
-        <v>0.53200000000000003</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="F16" s="7">
-        <v>0.504</v>
+        <v>0.52600000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -845,67 +833,67 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B24" s="7">
-        <v>0.871</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="C24" s="7">
-        <v>0.58499999999999996</v>
+        <v>0.91300000000000003</v>
       </c>
       <c r="D24" s="7">
-        <v>0.622</v>
+        <v>0.86699999999999999</v>
       </c>
       <c r="E24" s="9">
-        <v>0.58799999999999997</v>
+        <v>0.877</v>
       </c>
       <c r="F24" s="7">
-        <v>0.52400000000000002</v>
+        <v>0.86399999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B25" s="7">
-        <v>0.89200000000000002</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="C25" s="7">
-        <v>0.92</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="D25" s="7">
-        <v>0.24399999999999999</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="E25" s="10">
-        <v>0.35599999999999998</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="F25" s="7">
-        <v>0.40200000000000002</v>
+        <v>0.79500000000000004</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B26" s="7">
-        <v>0.82199999999999995</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="D26" s="7">
-        <v>0.24399999999999999</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="E26" s="11">
-        <v>0.35599999999999998</v>
+        <v>0.497</v>
       </c>
       <c r="F26" s="7">
-        <v>0.40200000000000002</v>
+        <v>0.52200000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B27">
         <v>0.92</v>
@@ -925,27 +913,27 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B28">
-        <v>0.91</v>
+        <v>0.89900000000000002</v>
       </c>
       <c r="C28" s="7">
-        <v>0.44400000000000001</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="D28" s="7">
-        <v>0.56100000000000005</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="E28" s="12">
-        <v>0.57599999999999996</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="F28" s="7">
-        <v>0.93100000000000005</v>
+        <v>0.57199999999999995</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -973,59 +961,59 @@
         <v>4</v>
       </c>
       <c r="B34">
-        <v>0.86499999999999999</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="C34">
-        <v>0.625</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="D34">
-        <v>0.55600000000000005</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="E34" s="1">
-        <v>0.56599999999999995</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="F34">
-        <v>0.502</v>
+        <v>0.76700000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B35">
-        <v>0.88900000000000001</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="C35">
-        <v>0.68600000000000005</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="D35">
-        <v>0.57799999999999996</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="E35" s="2">
-        <v>0.61299999999999999</v>
+        <v>0.88</v>
       </c>
       <c r="F35">
-        <v>0.56100000000000005</v>
+        <v>0.86399999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B36">
-        <v>0.92700000000000005</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="C36">
-        <v>0.82099999999999995</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="D36">
-        <v>0.71099999999999997</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="E36" s="3">
-        <v>0.751</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="F36">
-        <v>0.71799999999999997</v>
+        <v>0.51600000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1050,7 +1038,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B38">
         <v>0.91700000000000004</v>
@@ -1070,7 +1058,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1095,62 +1083,62 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B43">
-        <v>0.872</v>
+        <v>0.875</v>
       </c>
       <c r="C43">
-        <v>0.61199999999999999</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="D43">
-        <v>0.68899999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="E43" s="1">
-        <v>0.63500000000000001</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="F43">
-        <v>0.56899999999999995</v>
+        <v>0.52500000000000002</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B44">
-        <v>0.879</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="C44">
-        <v>0.61699999999999999</v>
+        <v>0.89400000000000002</v>
       </c>
       <c r="D44">
-        <v>0.64400000000000002</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="E44" s="2">
-        <v>0.60699999999999998</v>
+        <v>0.84199999999999997</v>
       </c>
       <c r="F44">
-        <v>0.55100000000000005</v>
+        <v>0.82399999999999995</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B45">
-        <v>0.94399999999999995</v>
+        <v>0.875</v>
       </c>
       <c r="C45">
-        <v>0.82399999999999995</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="D45">
-        <v>0.82199999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="E45" s="3">
-        <v>0.82199999999999995</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="F45">
-        <v>0.78900000000000003</v>
+        <v>0.52500000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1184,18 +1172,18 @@
         <v>0.871</v>
       </c>
       <c r="D47">
-        <v>0.6</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="E47" s="5">
-        <v>0.7</v>
+        <v>0.755</v>
       </c>
       <c r="F47">
-        <v>0.67700000000000005</v>
+        <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finalize - Update all scores
</commit_message>
<xml_diff>
--- a/FinalResult.xlsx
+++ b/FinalResult.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haha9\Documents\GitHub\quantum-flakiness-ml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB623DE-E2AB-4D41-BDC5-5BADBB29CE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1A9C18-E73C-4816-A485-E557C7D5DF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8385" yWindow="1920" windowWidth="17805" windowHeight="12780" xr2:uid="{0E69FEF2-CCF4-4F55-9C28-0EACB98F1DEB}"/>
+    <workbookView xWindow="7485" yWindow="1065" windowWidth="17805" windowHeight="12780" xr2:uid="{0E69FEF2-CCF4-4F55-9C28-0EACB98F1DEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$33:$L$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$28:$L$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>Model</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t xml:space="preserve"> XGBoost</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OriginThreshold </t>
+  </si>
+  <si>
+    <t>0.6,0.7</t>
+  </si>
+  <si>
+    <t>OriginalThreshold</t>
+  </si>
+  <si>
+    <t>0.5-0.9</t>
   </si>
 </sst>
 </file>
@@ -550,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31028914-FA6E-43D5-80A2-0461EDBCAA7F}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,12 +576,12 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -585,8 +600,14 @@
       <c r="F2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -605,8 +626,14 @@
       <c r="F3">
         <v>0.86299999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>0.1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -625,8 +652,14 @@
       <c r="F4">
         <v>0.82499999999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -645,8 +678,14 @@
       <c r="F5">
         <v>0.58599999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>0.7</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -665,8 +704,14 @@
       <c r="F6" s="7">
         <v>0.76800000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0.1</v>
+      </c>
+      <c r="H6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -685,13 +730,19 @@
       <c r="F7">
         <v>0.72499999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>0.4</v>
+      </c>
+      <c r="H7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -711,7 +762,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -731,7 +782,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -739,19 +790,19 @@
         <v>0.88900000000000001</v>
       </c>
       <c r="C13" s="7">
-        <v>0.88500000000000001</v>
+        <v>0.878</v>
       </c>
       <c r="D13" s="7">
         <v>0.91100000000000003</v>
       </c>
       <c r="E13" s="10">
-        <v>0.89300000000000002</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="F13" s="7">
-        <v>0.78800000000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.78600000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -771,7 +822,7 @@
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -791,7 +842,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -811,415 +862,451 @@
         <v>0.52600000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.877</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.86399999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.79500000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="C22">
+        <v>0.92</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="E22" s="11">
+        <v>0.497</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.52200000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>0.92</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="D23">
+        <v>0.622</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0.67200000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.57199999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C28" t="s">
         <v>8</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D28" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E28" t="s">
         <v>10</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F28" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="G28" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="7">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="C24" s="7">
-        <v>0.91300000000000003</v>
-      </c>
-      <c r="D24" s="7">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="E24" s="9">
-        <v>0.877</v>
-      </c>
-      <c r="F24" s="7">
+      <c r="B29">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="C29">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="D29">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="F29">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="G29">
+        <v>0.1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="C30">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="D30">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="F30">
         <v>0.86399999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="G30">
+        <v>0.5</v>
+      </c>
+      <c r="H30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>0.875</v>
+      </c>
+      <c r="C31">
+        <v>0.65</v>
+      </c>
+      <c r="D31">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="F31">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="G31">
+        <v>0.3</v>
+      </c>
+      <c r="H31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>0.92</v>
+      </c>
+      <c r="C32">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="D32">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="F32">
+        <v>0.69</v>
+      </c>
+      <c r="G32">
+        <v>0.2</v>
+      </c>
+      <c r="H32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>0.91</v>
+      </c>
+      <c r="C33">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="D33">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="F33">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="G33">
+        <v>0.1</v>
+      </c>
+      <c r="H33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="C38">
+        <v>0.91999999999999904</v>
+      </c>
+      <c r="D38">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="F38">
+        <v>0.84499999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="7">
-        <v>0.96099999999999997</v>
-      </c>
-      <c r="C25" s="7">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="D25" s="7">
-        <v>0.77800000000000002</v>
-      </c>
-      <c r="E25" s="10">
-        <v>0.86299999999999999</v>
-      </c>
-      <c r="F25" s="7">
-        <v>0.79500000000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B39">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="C39">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="D39">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="F39">
+        <v>0.82399999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="7">
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="C26">
+      <c r="B40">
+        <v>0.875</v>
+      </c>
+      <c r="C40">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="D40">
+        <v>0.6</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="F40">
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41">
         <v>0.92</v>
       </c>
-      <c r="D26" s="7">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="E26" s="11">
-        <v>0.497</v>
-      </c>
-      <c r="F26" s="7">
-        <v>0.52200000000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C41">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="D41">
+        <v>0.622</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="F41">
+        <v>0.67200000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>0.92</v>
+      </c>
+      <c r="C42">
+        <v>0.871</v>
+      </c>
+      <c r="D42">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="E42" s="5">
+        <v>0.755</v>
+      </c>
+      <c r="F42">
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B27">
-        <v>0.92</v>
-      </c>
-      <c r="C27" s="7">
-        <v>0.84499999999999997</v>
-      </c>
-      <c r="D27">
-        <v>0.622</v>
-      </c>
-      <c r="E27" s="4">
-        <v>0.69099999999999995</v>
-      </c>
-      <c r="F27" s="7">
-        <v>0.67200000000000004</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28">
-        <v>0.89900000000000002</v>
-      </c>
-      <c r="C28" s="7">
-        <v>0.84699999999999998</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="E28" s="12">
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="F28" s="7">
-        <v>0.57199999999999995</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="C34">
-        <v>0.73399999999999999</v>
-      </c>
-      <c r="D34">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="E34" s="1">
-        <v>0.80200000000000005</v>
-      </c>
-      <c r="F34">
-        <v>0.76700000000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35">
-        <v>0.96499999999999997</v>
-      </c>
-      <c r="C35">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="D35">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="E35" s="2">
-        <v>0.88</v>
-      </c>
-      <c r="F35">
-        <v>0.86399999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="C36">
-        <v>0.68600000000000005</v>
-      </c>
-      <c r="D36">
-        <v>0.57799999999999996</v>
-      </c>
-      <c r="E36" s="3">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="F36">
-        <v>0.51600000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="C37">
-        <v>0.77800000000000002</v>
-      </c>
-      <c r="D37">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="E37" s="4">
-        <v>0.747</v>
-      </c>
-      <c r="F37">
-        <v>0.71599999999999997</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="C38">
-        <v>0.77900000000000003</v>
-      </c>
-      <c r="D38">
-        <v>0.71099999999999997</v>
-      </c>
-      <c r="E38" s="5">
-        <v>0.73</v>
-      </c>
-      <c r="F38">
-        <v>0.69099999999999995</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>15</v>
-      </c>
-      <c r="B43">
-        <v>0.875</v>
-      </c>
-      <c r="C43">
-        <v>0.61099999999999999</v>
-      </c>
-      <c r="D43">
-        <v>0.6</v>
-      </c>
-      <c r="E43" s="1">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="F43">
-        <v>0.52500000000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44">
-        <v>0.95099999999999996</v>
-      </c>
-      <c r="C44">
-        <v>0.89400000000000002</v>
-      </c>
-      <c r="D44">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="E44" s="2">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="F44">
-        <v>0.82399999999999995</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45">
-        <v>0.875</v>
-      </c>
-      <c r="C45">
-        <v>0.61099999999999999</v>
-      </c>
-      <c r="D45">
-        <v>0.6</v>
-      </c>
-      <c r="E45" s="3">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="F45">
-        <v>0.52500000000000002</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46">
-        <v>0.92</v>
-      </c>
-      <c r="C46">
-        <v>0.84499999999999997</v>
-      </c>
-      <c r="D46">
-        <v>0.622</v>
-      </c>
-      <c r="E46" s="4">
-        <v>0.69099999999999995</v>
-      </c>
-      <c r="F46">
-        <v>0.67200000000000004</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B47">
-        <v>0.92</v>
-      </c>
-      <c r="C47">
-        <v>0.871</v>
-      </c>
-      <c r="D47">
-        <v>0.71099999999999997</v>
-      </c>
-      <c r="E47" s="5">
-        <v>0.755</v>
-      </c>
-      <c r="F47">
-        <v>0.72499999999999998</v>
-      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:L38">
-    <sortCondition ref="A34:A38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A29:L33">
+    <sortCondition ref="A29:A33"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>